<commit_message>
Minor changes in data files
</commit_message>
<xml_diff>
--- a/data/motors-deadzone/motors-deadzone_data.xlsx
+++ b/data/motors-deadzone/motors-deadzone_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inesctecpt-my.sharepoint.com/personal/ricardo_b_sousa_office365_inesctec_pt/Documents/inesctec/projects/trajectory-control/git/omni-control/src/data-processing/motors-deadzone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inesctecpt-my.sharepoint.com/personal/ricardo_b_sousa_office365_inesctec_pt/Documents/inesctec/projects/trajectory-control/git/omni-control/data/motors-deadzone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1425" documentId="11_F25DC773A252ABDACC1048E1099A4A345BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76C1FD75-2C3A-4DD5-B11B-5E5AEFCE0ECA}"/>
+  <xr:revisionPtr revIDLastSave="1427" documentId="11_F25DC773A252ABDACC1048E1099A4A345BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACF83388-BCB1-441C-8B8D-5A37A54F64DE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubber" sheetId="1" r:id="rId1"/>
@@ -3352,14 +3352,14 @@
     <mergeCell ref="J43:K43"/>
     <mergeCell ref="L43:M43"/>
     <mergeCell ref="N43:O43"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="R43:S43"/>
+    <mergeCell ref="T43:U43"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="F56:G56"/>
     <mergeCell ref="H56:I56"/>
     <mergeCell ref="J56:K56"/>
-    <mergeCell ref="P43:Q43"/>
-    <mergeCell ref="R43:S43"/>
-    <mergeCell ref="T43:U43"/>
     <mergeCell ref="L56:M56"/>
     <mergeCell ref="N56:O56"/>
     <mergeCell ref="P56:Q56"/>
@@ -5749,14 +5749,14 @@
     <mergeCell ref="J37:K37"/>
     <mergeCell ref="L37:M37"/>
     <mergeCell ref="N37:O37"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="T37:U37"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="F53:G53"/>
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="J53:K53"/>
-    <mergeCell ref="P37:Q37"/>
-    <mergeCell ref="R37:S37"/>
-    <mergeCell ref="T37:U37"/>
     <mergeCell ref="L53:M53"/>
     <mergeCell ref="N53:O53"/>
     <mergeCell ref="P53:Q53"/>
@@ -5771,7 +5771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44164C47-5158-4204-A274-8E19712A074E}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
@@ -5849,8 +5849,8 @@
         <v>28</v>
       </c>
       <c r="R5">
-        <f>MIN(G18:I18)*0.9</f>
-        <v>1.465875</v>
+        <f>MIN(G18:I18)*0.8</f>
+        <v>1.3029999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -5883,7 +5883,7 @@
       </c>
       <c r="R6">
         <f>R5*(1-0.6)</f>
-        <v>0.58635000000000004</v>
+        <v>0.5212</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>